<commit_message>
Started proper VNA schematic capture + new amp gerbers generated
</commit_message>
<xml_diff>
--- a/Hardware/Test Boards/BOM_Order_One.xlsx
+++ b/Hardware/Test Boards/BOM_Order_One.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\vna\Hardware\Test Boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C6D865-B82D-47EC-8AB1-1D0EA676FC48}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393D28FF-802E-4470-9A44-F88837B0048D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24750" xr2:uid="{856247D5-2B72-4218-AFEB-05CC3EC766DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{856247D5-2B72-4218-AFEB-05CC3EC766DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>820p</t>
   </si>
   <si>
-    <t>Bead 0402</t>
-  </si>
-  <si>
     <t>BLM18PG181SN1D</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/abracon-llc/ASTXR-12-19.200MHZ-512242-T/535-12687-1-ND/5017674</t>
+  </si>
+  <si>
+    <t>Bead 0603</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,10 +796,10 @@
         <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,13 +813,13 @@
         <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,13 +833,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
         <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,19 +847,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
         <v>77</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,10 +944,10 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
         <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,13 +1039,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,10 +1056,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1157,13 +1157,13 @@
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,19 +1171,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
         <v>89</v>
-      </c>
-      <c r="F26" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1211,13 +1211,13 @@
         <v>50</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" t="s">
         <v>83</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,13 +1231,13 @@
         <v>18</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" t="s">
         <v>85</v>
-      </c>
-      <c r="F29" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,13 +1251,13 @@
         <v>51</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" t="s">
         <v>87</v>
-      </c>
-      <c r="F30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,13 +1285,13 @@
         <v>49.9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
         <v>95</v>
-      </c>
-      <c r="F32" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,13 +1305,13 @@
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" t="s">
         <v>93</v>
-      </c>
-      <c r="F33" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1325,13 +1325,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
         <v>91</v>
-      </c>
-      <c r="F34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,13 +1345,13 @@
         <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" t="s">
         <v>97</v>
-      </c>
-      <c r="F35" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,13 +1365,13 @@
         <v>52.3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
         <v>99</v>
-      </c>
-      <c r="F36" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,13 +1385,13 @@
         <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" t="s">
         <v>107</v>
-      </c>
-      <c r="F37" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,16 +1402,16 @@
         <v>23</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
         <v>109</v>
-      </c>
-      <c r="F38" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1419,19 +1419,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="1">
         <v>90.9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" t="s">
         <v>101</v>
-      </c>
-      <c r="F39" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,19 +1439,19 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="1">
         <v>31.1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
         <v>103</v>
-      </c>
-      <c r="F40" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1459,19 +1459,19 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
         <v>105</v>
-      </c>
-      <c r="F41" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>15</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1499,13 +1499,13 @@
         <v>17</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" t="s">
         <v>111</v>
-      </c>
-      <c r="F43" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
         <v>16</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" t="s">
         <v>113</v>
-      </c>
-      <c r="F44" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1547,19 +1547,19 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
         <v>122</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>123</v>
-      </c>
-      <c r="F46" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,19 +1567,19 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" t="s">
         <v>117</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>118</v>
-      </c>
-      <c r="F47" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,19 +1587,19 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" t="s">
         <v>120</v>
-      </c>
-      <c r="F48" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>